<commit_message>
update timeline and scripts baudarate
</commit_message>
<xml_diff>
--- a/project Documentation/Second week/Second week Tasks and Timeline.xlsx
+++ b/project Documentation/Second week/Second week Tasks and Timeline.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>WEEK AT A GLANCE</t>
   </si>
@@ -164,6 +164,9 @@
   <si>
     <t>PI: (Return status xml)</t>
   </si>
+  <si>
+    <t>√</t>
+  </si>
 </sst>
 </file>
 
@@ -176,7 +179,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -621,7 +624,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -686,48 +689,32 @@
     <xf numFmtId="164" fontId="14" fillId="5" borderId="14" xfId="22" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="26">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="26">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="26" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="11" xfId="22" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="12" xfId="22" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="0" xfId="22" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="4" xfId="22" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="26" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="30">
@@ -2179,7 +2166,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>206528</xdr:colOff>
+      <xdr:colOff>206527</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>301724</xdr:rowOff>
     </xdr:to>
@@ -2198,7 +2185,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7081838" y="519978"/>
+          <a:off x="7593806" y="519978"/>
           <a:ext cx="363690" cy="281809"/>
           <a:chOff x="89" y="56"/>
           <a:chExt cx="781" cy="26"/>
@@ -2977,17 +2964,17 @@
   </sheetPr>
   <dimension ref="B1:J52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:H23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.7109375" customWidth="1"/>
     <col min="2" max="2" width="9.140625" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="70.42578125" customWidth="1"/>
+    <col min="5" max="5" width="78" customWidth="1"/>
     <col min="6" max="6" width="2.7109375" customWidth="1"/>
     <col min="7" max="7" width="3.28515625" customWidth="1"/>
     <col min="8" max="8" width="59.42578125" customWidth="1"/>
@@ -2995,8 +2982,8 @@
     <col min="10" max="10" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:10" ht="39.950000000000003" customHeight="1"/>
-    <row r="2" spans="3:10" ht="27.95" customHeight="1">
+    <row r="1" spans="3:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="3:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
@@ -3006,12 +2993,12 @@
         <v>1</v>
       </c>
       <c r="H2" s="6"/>
-      <c r="I2" s="29" t="s">
+      <c r="I2" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="29"/>
-    </row>
-    <row r="3" spans="3:10" ht="15" customHeight="1">
+      <c r="J2" s="20"/>
+    </row>
+    <row r="3" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="8" t="str">
         <f>IFERROR(TEXT(DATEVALUE(DateVal)+1,"dddd"),"")</f>
         <v/>
@@ -3021,37 +3008,39 @@
       </c>
       <c r="E3" s="15"/>
       <c r="G3" s="10"/>
-      <c r="H3" s="31" t="s">
+      <c r="H3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="30"/>
-    </row>
-    <row r="4" spans="3:10" ht="15" customHeight="1">
-      <c r="C4" s="20">
+      <c r="J3" s="22"/>
+    </row>
+    <row r="4" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="25">
         <v>43984</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="17"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-    </row>
-    <row r="5" spans="3:10" ht="15" customHeight="1">
-      <c r="C5" s="21"/>
+      <c r="G4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="27"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+    </row>
+    <row r="5" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="26"/>
       <c r="D5" s="16"/>
       <c r="E5" s="17"/>
       <c r="G5" s="11"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-    </row>
-    <row r="6" spans="3:10" ht="15" customHeight="1">
+      <c r="H5" s="27"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+    </row>
+    <row r="6" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="str">
         <f>IFERROR(DateVal+1,"")</f>
         <v/>
@@ -3059,35 +3048,37 @@
       <c r="D6" s="16"/>
       <c r="E6" s="17"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="32" t="s">
+      <c r="I6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="28"/>
-    </row>
-    <row r="7" spans="3:10" ht="15" customHeight="1">
+      <c r="J6" s="23"/>
+    </row>
+    <row r="7" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="17"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-    </row>
-    <row r="8" spans="3:10" ht="15" customHeight="1">
+      <c r="G7" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="24"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+    </row>
+    <row r="8" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
       <c r="D8" s="18"/>
       <c r="E8" s="19"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-    </row>
-    <row r="9" spans="3:10" ht="15" customHeight="1">
+      <c r="H8" s="24"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+    </row>
+    <row r="9" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="str">
         <f>IFERROR(TEXT(DATEVALUE(DateVal)+2,"dddd"),"")</f>
         <v/>
@@ -3097,39 +3088,41 @@
       </c>
       <c r="E9" s="15"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="31" t="s">
+      <c r="H9" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="32" t="s">
+      <c r="I9" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="28"/>
-    </row>
-    <row r="10" spans="3:10" ht="15" customHeight="1">
-      <c r="C10" s="20">
+      <c r="J9" s="23"/>
+    </row>
+    <row r="10" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="25">
         <v>43985</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="17"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-    </row>
-    <row r="11" spans="3:10" ht="15" customHeight="1">
-      <c r="C11" s="21"/>
+      <c r="G10" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="24"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+    </row>
+    <row r="11" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="26"/>
       <c r="D11" s="16" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="17"/>
       <c r="G11" s="11"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-    </row>
-    <row r="12" spans="3:10" ht="15" customHeight="1">
+      <c r="H11" s="24"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+    </row>
+    <row r="12" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="str">
         <f>IFERROR(DateVal+2,"")</f>
         <v/>
@@ -3139,35 +3132,35 @@
       </c>
       <c r="E12" s="17"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="28" t="s">
+      <c r="I12" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="28"/>
-    </row>
-    <row r="13" spans="3:10" ht="15" customHeight="1">
+      <c r="J12" s="23"/>
+    </row>
+    <row r="13" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="17"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-    </row>
-    <row r="14" spans="3:10" ht="15" customHeight="1">
+      <c r="H13" s="24"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+    </row>
+    <row r="14" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
       <c r="D14" s="18"/>
       <c r="E14" s="19"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-    </row>
-    <row r="15" spans="3:10" ht="15" customHeight="1">
+      <c r="H14" s="24"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+    </row>
+    <row r="15" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="8" t="str">
         <f>IFERROR(TEXT(DATEVALUE(DateVal)+3,"dddd"),"")</f>
         <v/>
@@ -3177,16 +3170,16 @@
       </c>
       <c r="E15" s="15"/>
       <c r="G15" s="9"/>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="28" t="s">
+      <c r="I15" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="28"/>
-    </row>
-    <row r="16" spans="3:10" ht="15" customHeight="1">
-      <c r="C16" s="20">
+      <c r="J15" s="23"/>
+    </row>
+    <row r="16" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="25">
         <v>43986</v>
       </c>
       <c r="D16" s="16" t="s">
@@ -3194,22 +3187,22 @@
       </c>
       <c r="E16" s="17"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-    </row>
-    <row r="17" spans="3:10" ht="15" customHeight="1">
-      <c r="C17" s="21"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+    </row>
+    <row r="17" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="26"/>
       <c r="D17" s="16" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="17"/>
       <c r="G17" s="11"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-    </row>
-    <row r="18" spans="3:10" ht="15" customHeight="1">
+      <c r="H17" s="24"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+    </row>
+    <row r="18" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="str">
         <f>IFERROR(DateVal+3,"")</f>
         <v/>
@@ -3217,35 +3210,35 @@
       <c r="D18" s="16"/>
       <c r="E18" s="17"/>
       <c r="G18" s="9"/>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I18" s="28" t="s">
+      <c r="I18" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="28"/>
-    </row>
-    <row r="19" spans="3:10" ht="15" customHeight="1">
+      <c r="J18" s="22"/>
+    </row>
+    <row r="19" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="17"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-    </row>
-    <row r="20" spans="3:10" ht="15" customHeight="1">
+      <c r="H19" s="27"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+    </row>
+    <row r="20" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="2"/>
       <c r="D20" s="18"/>
       <c r="E20" s="19"/>
       <c r="G20" s="11"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-    </row>
-    <row r="21" spans="3:10" ht="15" customHeight="1">
+      <c r="H20" s="27"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+    </row>
+    <row r="21" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="8" t="str">
         <f>IFERROR(TEXT(DATEVALUE(DateVal)+4,"dddd"),"")</f>
         <v/>
@@ -3255,16 +3248,16 @@
       </c>
       <c r="E21" s="15"/>
       <c r="G21" s="9"/>
-      <c r="H21" s="23" t="s">
+      <c r="H21" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="I21" s="28" t="s">
+      <c r="I21" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="J21" s="28"/>
-    </row>
-    <row r="22" spans="3:10" ht="15" customHeight="1">
-      <c r="C22" s="20">
+      <c r="J21" s="22"/>
+    </row>
+    <row r="22" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="25">
         <v>43987</v>
       </c>
       <c r="D22" s="16" t="s">
@@ -3272,22 +3265,22 @@
       </c>
       <c r="E22" s="17"/>
       <c r="G22" s="7"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-    </row>
-    <row r="23" spans="3:10" ht="15" customHeight="1">
-      <c r="C23" s="21"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+    </row>
+    <row r="23" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="26"/>
       <c r="D23" s="16" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="17"/>
       <c r="G23" s="11"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-    </row>
-    <row r="24" spans="3:10" ht="15" customHeight="1">
+      <c r="H23" s="24"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+    </row>
+    <row r="24" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="12" t="s">
         <v>5</v>
       </c>
@@ -3296,274 +3289,281 @@
       </c>
       <c r="E24" s="17"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="23" t="s">
+      <c r="H24" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="I24" s="28" t="s">
+      <c r="I24" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="J24" s="28"/>
-    </row>
-    <row r="25" spans="3:10" ht="15" customHeight="1">
+      <c r="J24" s="22"/>
+    </row>
+    <row r="25" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="2"/>
       <c r="D25" s="18"/>
       <c r="E25" s="19"/>
       <c r="G25" s="7"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-    </row>
-    <row r="26" spans="3:10" ht="15" customHeight="1">
+      <c r="H25" s="24"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+    </row>
+    <row r="26" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="8" t="str">
         <f>IFERROR(TEXT(DATEVALUE(DateVal)+5,"dddd"),"")</f>
         <v/>
       </c>
       <c r="E26" s="15"/>
       <c r="G26" s="11"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-    </row>
-    <row r="27" spans="3:10" ht="15" customHeight="1">
-      <c r="C27" s="20">
+      <c r="H26" s="24"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+    </row>
+    <row r="27" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="25">
         <v>43988</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="17"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="22" t="s">
+      <c r="H27" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="I27" s="28" t="s">
+      <c r="I27" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="J27" s="28"/>
-    </row>
-    <row r="28" spans="3:10" ht="15" customHeight="1">
-      <c r="C28" s="21"/>
+      <c r="J27" s="23"/>
+    </row>
+    <row r="28" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="26"/>
       <c r="D28" s="16"/>
       <c r="E28" s="17"/>
       <c r="G28" s="7"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-    </row>
-    <row r="29" spans="3:10" ht="15" customHeight="1">
+      <c r="H28" s="24"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+    </row>
+    <row r="29" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="17"/>
       <c r="G29" s="11"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-    </row>
-    <row r="30" spans="3:10" ht="15" customHeight="1">
+      <c r="H29" s="24"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+    </row>
+    <row r="30" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="2"/>
       <c r="D30" s="18"/>
       <c r="E30" s="19"/>
       <c r="G30" s="9"/>
-      <c r="H30" s="22" t="s">
+      <c r="H30" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I30" s="28" t="s">
+      <c r="I30" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="J30" s="28"/>
-    </row>
-    <row r="31" spans="3:10" ht="15" customHeight="1">
+      <c r="J30" s="21"/>
+    </row>
+    <row r="31" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C31" s="8" t="str">
         <f>IFERROR(TEXT(DATEVALUE(DateVal)+6,"dddd"),"")</f>
         <v/>
       </c>
-      <c r="D31" s="24" t="str">
+      <c r="D31" s="14" t="str">
         <f>IFERROR(INDEX(#REF!,MATCH($C$34&amp;"|"&amp;ROW(A1),#REF!,0),2),"")</f>
         <v/>
       </c>
-      <c r="E31" s="25"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="28"/>
-    </row>
-    <row r="32" spans="3:10" ht="15" customHeight="1">
-      <c r="C32" s="20">
+      <c r="E31" s="15"/>
+      <c r="G31" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H31" s="28"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+    </row>
+    <row r="32" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="25">
         <v>43989</v>
       </c>
-      <c r="D32" s="26"/>
-      <c r="E32" s="27"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="17"/>
       <c r="G32" s="11"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="28"/>
-    </row>
-    <row r="33" spans="3:10" ht="15" customHeight="1">
-      <c r="C33" s="21"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="27"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+    </row>
+    <row r="33" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="26"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="17"/>
       <c r="G33" s="9"/>
-      <c r="H33" s="22" t="s">
+      <c r="H33" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="I33" s="28" t="s">
+      <c r="I33" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="J33" s="28"/>
-    </row>
-    <row r="34" spans="3:10" ht="15" customHeight="1">
+      <c r="J33" s="23"/>
+    </row>
+    <row r="34" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="26"/>
-      <c r="E34" s="27"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="17"/>
       <c r="G34" s="7"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="28"/>
-    </row>
-    <row r="35" spans="3:10" ht="15" customHeight="1">
+      <c r="H34" s="24"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+    </row>
+    <row r="35" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="2"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="27"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="17"/>
       <c r="G35" s="11"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="28"/>
-    </row>
-    <row r="36" spans="3:10" ht="15" customHeight="1">
+      <c r="H35" s="24"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+    </row>
+    <row r="36" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G36" s="10"/>
-      <c r="H36" s="23" t="s">
+      <c r="H36" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="I36" s="30" t="s">
+      <c r="I36" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J36" s="30"/>
-    </row>
-    <row r="37" spans="3:10" ht="13.5" customHeight="1">
+      <c r="J36" s="22"/>
+    </row>
+    <row r="37" spans="3:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G37" s="7"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
-    </row>
-    <row r="38" spans="3:10" ht="23.25">
+      <c r="H37" s="27"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+    </row>
+    <row r="38" spans="3:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="G38" s="11"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="30"/>
-    </row>
-    <row r="39" spans="3:10">
+      <c r="H38" s="27"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F39" s="4"/>
       <c r="G39" s="10"/>
-      <c r="H39" s="22" t="s">
+      <c r="H39" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="I39" s="28" t="s">
+      <c r="I39" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="J39" s="28"/>
-    </row>
-    <row r="40" spans="3:10" ht="15" customHeight="1">
+      <c r="J39" s="23"/>
+    </row>
+    <row r="40" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F40" s="4"/>
       <c r="G40" s="7"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="28"/>
-    </row>
-    <row r="41" spans="3:10" ht="23.25">
+      <c r="H40" s="24"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="23"/>
+    </row>
+    <row r="41" spans="3:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="F41" s="4"/>
       <c r="G41" s="11"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="28"/>
-      <c r="J41" s="28"/>
-    </row>
-    <row r="42" spans="3:10">
+      <c r="H41" s="24"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="23"/>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F42" s="4"/>
       <c r="G42" s="10"/>
-      <c r="H42" s="22" t="s">
+      <c r="H42" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="I42" s="28" t="s">
+      <c r="I42" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="J42" s="28"/>
-    </row>
-    <row r="43" spans="3:10" ht="14.25" customHeight="1">
+      <c r="J42" s="23"/>
+    </row>
+    <row r="43" spans="3:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F43" s="4"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="28"/>
-      <c r="J43" s="28"/>
-    </row>
-    <row r="44" spans="3:10" ht="23.25">
+      <c r="H43" s="24"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
+    </row>
+    <row r="44" spans="3:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="F44" s="4"/>
       <c r="G44" s="11"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="28"/>
-      <c r="J44" s="28"/>
-    </row>
-    <row r="45" spans="3:10">
+      <c r="H44" s="24"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
+    </row>
+    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F45" s="4"/>
       <c r="G45" s="10"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="I45" s="28" t="s">
+      <c r="I45" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="J45" s="28"/>
-    </row>
-    <row r="46" spans="3:10" ht="15.75" customHeight="1">
+      <c r="J45" s="23"/>
+    </row>
+    <row r="46" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F46" s="4"/>
       <c r="G46" s="7"/>
-      <c r="H46" s="22"/>
-      <c r="I46" s="28"/>
-      <c r="J46" s="28"/>
-    </row>
-    <row r="47" spans="3:10" ht="23.25">
+      <c r="H46" s="24"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="23"/>
+    </row>
+    <row r="47" spans="3:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="F47" s="4"/>
       <c r="G47" s="11"/>
-      <c r="H47" s="22"/>
-      <c r="I47" s="28"/>
-      <c r="J47" s="28"/>
-    </row>
-    <row r="48" spans="3:10">
+      <c r="H47" s="24"/>
+      <c r="I47" s="23"/>
+      <c r="J47" s="23"/>
+    </row>
+    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G48" s="10"/>
-      <c r="H48" s="22" t="s">
+      <c r="H48" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="I48" s="28" t="s">
+      <c r="I48" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="J48" s="28"/>
-    </row>
-    <row r="49" spans="7:10" ht="15.75" customHeight="1">
+      <c r="J48" s="23"/>
+    </row>
+    <row r="49" spans="7:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G49" s="7"/>
-      <c r="H49" s="22"/>
-      <c r="I49" s="28"/>
-      <c r="J49" s="28"/>
-    </row>
-    <row r="50" spans="7:10" ht="23.25">
+      <c r="H49" s="24"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="23"/>
+    </row>
+    <row r="50" spans="7:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="G50" s="11"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="28"/>
-      <c r="J50" s="28"/>
-    </row>
-    <row r="51" spans="7:10" ht="15" customHeight="1"/>
-    <row r="52" spans="7:10" ht="15" customHeight="1"/>
+      <c r="H50" s="24"/>
+      <c r="I50" s="23"/>
+      <c r="J50" s="23"/>
+    </row>
+    <row r="51" spans="7:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="7:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J5"/>
-    <mergeCell ref="I6:J8"/>
-    <mergeCell ref="I9:J11"/>
-    <mergeCell ref="I12:J14"/>
-    <mergeCell ref="H42:H44"/>
-    <mergeCell ref="I42:J44"/>
-    <mergeCell ref="I45:J47"/>
-    <mergeCell ref="I48:J50"/>
-    <mergeCell ref="H48:H50"/>
+  <mergeCells count="39">
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="H45:H47"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="H33:H35"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="H27:H29"/>
+    <mergeCell ref="H30:H32"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="C22:C23"/>
@@ -3578,22 +3578,16 @@
     <mergeCell ref="I27:J29"/>
     <mergeCell ref="I30:J32"/>
     <mergeCell ref="I36:J38"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="H45:H47"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="H33:H35"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="D31:E35"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="H27:H29"/>
-    <mergeCell ref="H30:H32"/>
+    <mergeCell ref="H42:H44"/>
+    <mergeCell ref="I42:J44"/>
+    <mergeCell ref="I45:J47"/>
+    <mergeCell ref="I48:J50"/>
+    <mergeCell ref="H48:H50"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J5"/>
+    <mergeCell ref="I6:J8"/>
+    <mergeCell ref="I9:J11"/>
+    <mergeCell ref="I12:J14"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Notes or To Do list in this column" sqref="H2"/>
@@ -3626,15 +3620,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a8a52e8c320b9a064ae3583ae3861c92">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88020cb39231a0945110f9cd888b521a" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -3855,6 +3840,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71FCDC0B-BE17-4EFD-AAD5-1E4E9349882C}">
   <ds:schemaRefs>
@@ -3873,14 +3867,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19F07B9F-2027-487B-9D1F-78CE832B31AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47490C6C-6B46-4DFD-9ACA-031AB2832B8C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3897,4 +3883,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19F07B9F-2027-487B-9D1F-78CE832B31AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Timeline & tasks update
Finishing bootloadeer tasks
</commit_message>
<xml_diff>
--- a/project Documentation/Second week/Second week Tasks and Timeline.xlsx
+++ b/project Documentation/Second week/Second week Tasks and Timeline.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
   <si>
     <t>WEEK AT A GLANCE</t>
   </si>
@@ -689,32 +689,32 @@
     <xf numFmtId="164" fontId="14" fillId="5" borderId="14" xfId="22" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="16" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="26" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="26" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="26">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="26">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="26" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="26" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="30">
@@ -2964,8 +2964,8 @@
   </sheetPr>
   <dimension ref="B1:J52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2993,10 +2993,10 @@
         <v>1</v>
       </c>
       <c r="H2" s="6"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="20"/>
+      <c r="J2" s="28"/>
     </row>
     <row r="3" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="8" t="str">
@@ -3008,16 +3008,16 @@
       </c>
       <c r="E3" s="15"/>
       <c r="G3" s="10"/>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="22"/>
+      <c r="J3" s="26"/>
     </row>
     <row r="4" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="25">
+      <c r="C4" s="20">
         <v>43984</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -3027,18 +3027,18 @@
       <c r="G4" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="27"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
     </row>
     <row r="5" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="26"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="16"/>
       <c r="E5" s="17"/>
       <c r="G5" s="11"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
     </row>
     <row r="6" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="str">
@@ -3048,13 +3048,13 @@
       <c r="D6" s="16"/>
       <c r="E6" s="17"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="28" t="s">
+      <c r="H6" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="23"/>
+      <c r="J6" s="25"/>
     </row>
     <row r="7" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
@@ -3066,8 +3066,8 @@
         <v>33</v>
       </c>
       <c r="H7" s="24"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
     </row>
     <row r="8" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
@@ -3075,8 +3075,8 @@
       <c r="E8" s="19"/>
       <c r="G8" s="11"/>
       <c r="H8" s="24"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
     </row>
     <row r="9" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="str">
@@ -3088,16 +3088,16 @@
       </c>
       <c r="E9" s="15"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="28" t="s">
+      <c r="H9" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="23"/>
+      <c r="J9" s="25"/>
     </row>
     <row r="10" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="25">
+      <c r="C10" s="20">
         <v>43985</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -3108,19 +3108,19 @@
         <v>33</v>
       </c>
       <c r="H10" s="24"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
     </row>
     <row r="11" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="26"/>
+      <c r="C11" s="21"/>
       <c r="D11" s="16" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="17"/>
       <c r="G11" s="11"/>
       <c r="H11" s="24"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
     </row>
     <row r="12" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="str">
@@ -3135,10 +3135,10 @@
       <c r="H12" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="23" t="s">
+      <c r="I12" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="23"/>
+      <c r="J12" s="25"/>
     </row>
     <row r="13" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
@@ -3148,8 +3148,8 @@
       <c r="E13" s="17"/>
       <c r="G13" s="7"/>
       <c r="H13" s="24"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
     </row>
     <row r="14" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
@@ -3157,8 +3157,8 @@
       <c r="E14" s="19"/>
       <c r="G14" s="11"/>
       <c r="H14" s="24"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
     </row>
     <row r="15" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="8" t="str">
@@ -3173,13 +3173,13 @@
       <c r="H15" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="23" t="s">
+      <c r="I15" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="23"/>
+      <c r="J15" s="25"/>
     </row>
     <row r="16" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="25">
+      <c r="C16" s="20">
         <v>43986</v>
       </c>
       <c r="D16" s="16" t="s">
@@ -3188,19 +3188,19 @@
       <c r="E16" s="17"/>
       <c r="G16" s="7"/>
       <c r="H16" s="24"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
     </row>
     <row r="17" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="26"/>
+      <c r="C17" s="21"/>
       <c r="D17" s="16" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="17"/>
       <c r="G17" s="11"/>
       <c r="H17" s="24"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
     </row>
     <row r="18" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="str">
@@ -3210,13 +3210,13 @@
       <c r="D18" s="16"/>
       <c r="E18" s="17"/>
       <c r="G18" s="9"/>
-      <c r="H18" s="27" t="s">
+      <c r="H18" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I18" s="22" t="s">
+      <c r="I18" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="22"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
@@ -3225,18 +3225,18 @@
       <c r="D19" s="16"/>
       <c r="E19" s="17"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
     </row>
     <row r="20" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="2"/>
       <c r="D20" s="18"/>
       <c r="E20" s="19"/>
       <c r="G20" s="11"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="8" t="str">
@@ -3248,16 +3248,16 @@
       </c>
       <c r="E21" s="15"/>
       <c r="G21" s="9"/>
-      <c r="H21" s="27" t="s">
+      <c r="H21" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="I21" s="22" t="s">
+      <c r="I21" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="J21" s="22"/>
+      <c r="J21" s="26"/>
     </row>
     <row r="22" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="25">
+      <c r="C22" s="20">
         <v>43987</v>
       </c>
       <c r="D22" s="16" t="s">
@@ -3266,19 +3266,19 @@
       <c r="E22" s="17"/>
       <c r="G22" s="7"/>
       <c r="H22" s="24"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
     </row>
     <row r="23" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="26"/>
+      <c r="C23" s="21"/>
       <c r="D23" s="16" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="17"/>
       <c r="G23" s="11"/>
       <c r="H23" s="24"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
     </row>
     <row r="24" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="12" t="s">
@@ -3289,13 +3289,13 @@
       </c>
       <c r="E24" s="17"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="27" t="s">
+      <c r="H24" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I24" s="22" t="s">
+      <c r="I24" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="J24" s="22"/>
+      <c r="J24" s="26"/>
     </row>
     <row r="25" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="2"/>
@@ -3303,8 +3303,8 @@
       <c r="E25" s="19"/>
       <c r="G25" s="7"/>
       <c r="H25" s="24"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
     </row>
     <row r="26" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="8" t="str">
@@ -3314,11 +3314,11 @@
       <c r="E26" s="15"/>
       <c r="G26" s="11"/>
       <c r="H26" s="24"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
     </row>
     <row r="27" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="25">
+      <c r="C27" s="20">
         <v>43988</v>
       </c>
       <c r="D27" s="16"/>
@@ -3327,19 +3327,19 @@
       <c r="H27" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="I27" s="23" t="s">
+      <c r="I27" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J27" s="23"/>
+      <c r="J27" s="25"/>
     </row>
     <row r="28" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="26"/>
+      <c r="C28" s="21"/>
       <c r="D28" s="16"/>
       <c r="E28" s="17"/>
       <c r="G28" s="7"/>
       <c r="H28" s="24"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="12" t="s">
@@ -3349,21 +3349,21 @@
       <c r="E29" s="17"/>
       <c r="G29" s="11"/>
       <c r="H29" s="24"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="2"/>
       <c r="D30" s="18"/>
       <c r="E30" s="19"/>
       <c r="G30" s="9"/>
-      <c r="H30" s="28" t="s">
+      <c r="H30" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="I30" s="21" t="s">
+      <c r="I30" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="J30" s="21"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C31" s="8" t="str">
@@ -3378,33 +3378,33 @@
       <c r="G31" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H31" s="28"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="32" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="25">
+      <c r="C32" s="20">
         <v>43989</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="17"/>
       <c r="G32" s="11"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="27"/>
     </row>
     <row r="33" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="26"/>
+      <c r="C33" s="21"/>
       <c r="D33" s="16"/>
       <c r="E33" s="17"/>
       <c r="G33" s="9"/>
       <c r="H33" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="I33" s="23" t="s">
+      <c r="I33" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="J33" s="23"/>
+      <c r="J33" s="25"/>
     </row>
     <row r="34" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="12" t="s">
@@ -3414,8 +3414,8 @@
       <c r="E34" s="17"/>
       <c r="G34" s="7"/>
       <c r="H34" s="24"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="23"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
     </row>
     <row r="35" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="2"/>
@@ -3423,132 +3423,161 @@
       <c r="E35" s="17"/>
       <c r="G35" s="11"/>
       <c r="H35" s="24"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="23"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="25"/>
     </row>
     <row r="36" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G36" s="10"/>
-      <c r="H36" s="27" t="s">
+      <c r="H36" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="I36" s="22" t="s">
+      <c r="I36" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="J36" s="22"/>
+      <c r="J36" s="26"/>
     </row>
     <row r="37" spans="3:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G37" s="7"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
     </row>
     <row r="38" spans="3:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="G38" s="11"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
     </row>
     <row r="39" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F39" s="4"/>
       <c r="G39" s="10"/>
-      <c r="H39" s="24" t="s">
+      <c r="H39" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="I39" s="23" t="s">
+      <c r="I39" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="J39" s="23"/>
+      <c r="J39" s="27"/>
     </row>
     <row r="40" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F40" s="4"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="23"/>
-      <c r="J40" s="23"/>
+      <c r="G40" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H40" s="23"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27"/>
     </row>
     <row r="41" spans="3:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="F41" s="4"/>
       <c r="G41" s="11"/>
-      <c r="H41" s="24"/>
-      <c r="I41" s="23"/>
-      <c r="J41" s="23"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="27"/>
     </row>
     <row r="42" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F42" s="4"/>
       <c r="G42" s="10"/>
-      <c r="H42" s="24" t="s">
+      <c r="H42" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="I42" s="23" t="s">
+      <c r="I42" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="J42" s="23"/>
+      <c r="J42" s="27"/>
     </row>
     <row r="43" spans="3:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F43" s="4"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="G43" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H43" s="23"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
     </row>
     <row r="44" spans="3:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="F44" s="4"/>
       <c r="G44" s="11"/>
-      <c r="H44" s="24"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F45" s="4"/>
       <c r="G45" s="10"/>
-      <c r="H45" s="24" t="s">
+      <c r="H45" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I45" s="23" t="s">
+      <c r="I45" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="J45" s="23"/>
+      <c r="J45" s="27"/>
     </row>
     <row r="46" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F46" s="4"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="23"/>
-      <c r="J46" s="23"/>
+      <c r="G46" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H46" s="23"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
     </row>
     <row r="47" spans="3:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="F47" s="4"/>
       <c r="G47" s="11"/>
-      <c r="H47" s="24"/>
-      <c r="I47" s="23"/>
-      <c r="J47" s="23"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="27"/>
+      <c r="J47" s="27"/>
     </row>
     <row r="48" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G48" s="10"/>
       <c r="H48" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="I48" s="23" t="s">
+      <c r="I48" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="J48" s="23"/>
+      <c r="J48" s="25"/>
     </row>
     <row r="49" spans="7:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G49" s="7"/>
       <c r="H49" s="24"/>
-      <c r="I49" s="23"/>
-      <c r="J49" s="23"/>
+      <c r="I49" s="25"/>
+      <c r="J49" s="25"/>
     </row>
     <row r="50" spans="7:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="G50" s="11"/>
       <c r="H50" s="24"/>
-      <c r="I50" s="23"/>
-      <c r="J50" s="23"/>
+      <c r="I50" s="25"/>
+      <c r="J50" s="25"/>
     </row>
     <row r="51" spans="7:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="52" spans="7:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J5"/>
+    <mergeCell ref="I6:J8"/>
+    <mergeCell ref="I9:J11"/>
+    <mergeCell ref="I12:J14"/>
+    <mergeCell ref="H42:H44"/>
+    <mergeCell ref="I42:J44"/>
+    <mergeCell ref="I45:J47"/>
+    <mergeCell ref="I48:J50"/>
+    <mergeCell ref="H48:H50"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="I33:J35"/>
+    <mergeCell ref="I39:J41"/>
+    <mergeCell ref="H36:H38"/>
+    <mergeCell ref="H39:H41"/>
+    <mergeCell ref="I18:J20"/>
+    <mergeCell ref="I15:J17"/>
+    <mergeCell ref="I21:J23"/>
+    <mergeCell ref="I24:J26"/>
+    <mergeCell ref="I27:J29"/>
+    <mergeCell ref="I30:J32"/>
+    <mergeCell ref="I36:J38"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="H18:H20"/>
     <mergeCell ref="H3:H5"/>
@@ -3565,29 +3594,6 @@
     <mergeCell ref="H27:H29"/>
     <mergeCell ref="H30:H32"/>
     <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="I33:J35"/>
-    <mergeCell ref="I39:J41"/>
-    <mergeCell ref="H36:H38"/>
-    <mergeCell ref="H39:H41"/>
-    <mergeCell ref="I18:J20"/>
-    <mergeCell ref="I15:J17"/>
-    <mergeCell ref="I21:J23"/>
-    <mergeCell ref="I24:J26"/>
-    <mergeCell ref="I27:J29"/>
-    <mergeCell ref="I30:J32"/>
-    <mergeCell ref="I36:J38"/>
-    <mergeCell ref="H42:H44"/>
-    <mergeCell ref="I42:J44"/>
-    <mergeCell ref="I45:J47"/>
-    <mergeCell ref="I48:J50"/>
-    <mergeCell ref="H48:H50"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J5"/>
-    <mergeCell ref="I6:J8"/>
-    <mergeCell ref="I9:J11"/>
-    <mergeCell ref="I12:J14"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Notes or To Do list in this column" sqref="H2"/>
@@ -3620,6 +3626,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a8a52e8c320b9a064ae3583ae3861c92">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88020cb39231a0945110f9cd888b521a" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -3840,15 +3855,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71FCDC0B-BE17-4EFD-AAD5-1E4E9349882C}">
   <ds:schemaRefs>
@@ -3867,6 +3873,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19F07B9F-2027-487B-9D1F-78CE832B31AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47490C6C-6B46-4DFD-9ACA-031AB2832B8C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3883,12 +3897,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19F07B9F-2027-487B-9D1F-78CE832B31AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
plan updating Signed-off-by: MarcelleSamir <marcelle.samir.s@gmail.com>
</commit_message>
<xml_diff>
--- a/project Documentation/Second week/Second week Tasks and Timeline.xlsx
+++ b/project Documentation/Second week/Second week Tasks and Timeline.xlsx
@@ -74,28 +74,6 @@
     <t>XML parser and change Request.txt to XML file</t>
   </si>
   <si>
-    <r>
-      <t>After uploading file: (Report load successfully - Wait for 1 min for a flashing report from R</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>π</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Segoe Print"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t>Button check last file status (Activated after Timeout)</t>
   </si>
   <si>
@@ -106,9 +84,6 @@
   </si>
   <si>
     <t>Python GUI error handling (check .elf file &amp; not empty - upload file exceptions)</t>
-  </si>
-  <si>
-    <t>PI: (Return status)</t>
   </si>
   <si>
     <t>PI: (GUI Interaction)</t>
@@ -164,6 +139,31 @@
   <si>
     <t>After uploading file: (Report load successfully - Wait for 1 min for a flashing report from Rπ)</t>
   </si>
+  <si>
+    <r>
+      <t>After uploading file: (Report load successfully - Wait for 1 min for a flashing report from R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="6" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>π</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="6" tint="0.39997558519241921"/>
+        <rFont val="Segoe Print"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>PI: (Return status xml)</t>
+  </si>
 </sst>
 </file>
 
@@ -176,7 +176,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,6 +317,17 @@
       <sz val="11"/>
       <color rgb="FFEE7748"/>
       <name val="Segoe Print"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="0.39997558519241921"/>
+      <name val="Segoe Print"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -610,7 +621,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -675,20 +686,17 @@
     <xf numFmtId="164" fontId="14" fillId="5" borderId="14" xfId="22" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="16" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="26">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="26" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="5" borderId="11" xfId="22" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -706,10 +714,19 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="26" applyFont="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="26" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -982,7 +999,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="209334" y="534265"/>
+          <a:off x="214097" y="529503"/>
           <a:ext cx="432547" cy="292763"/>
           <a:chOff x="306" y="55"/>
           <a:chExt cx="291" cy="27"/>
@@ -2181,8 +2198,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7086600" y="524740"/>
-          <a:ext cx="368453" cy="281809"/>
+          <a:off x="7081838" y="519978"/>
+          <a:ext cx="363690" cy="281809"/>
           <a:chOff x="89" y="56"/>
           <a:chExt cx="781" cy="26"/>
         </a:xfrm>
@@ -2960,11 +2977,11 @@
   </sheetPr>
   <dimension ref="B1:J52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39:H41"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21:H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="1.7109375" customWidth="1"/>
     <col min="2" max="2" width="9.140625" hidden="1" customWidth="1"/>
@@ -2978,8 +2995,8 @@
     <col min="10" max="10" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="3:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:10" ht="39.950000000000003" customHeight="1"/>
+    <row r="2" spans="3:10" ht="27.95" customHeight="1">
       <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
@@ -2989,12 +3006,12 @@
         <v>1</v>
       </c>
       <c r="H2" s="6"/>
-      <c r="I2" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="22"/>
-    </row>
-    <row r="3" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="29"/>
+    </row>
+    <row r="3" spans="3:10" ht="15" customHeight="1">
       <c r="C3" s="8" t="str">
         <f>IFERROR(TEXT(DATEVALUE(DateVal)+1,"dddd"),"")</f>
         <v/>
@@ -3004,37 +3021,37 @@
       </c>
       <c r="E3" s="15"/>
       <c r="G3" s="10"/>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="30" t="s">
-        <v>25</v>
+      <c r="I3" s="32" t="s">
+        <v>23</v>
       </c>
       <c r="J3" s="30"/>
     </row>
-    <row r="4" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="23">
+    <row r="4" spans="3:10" ht="15" customHeight="1">
+      <c r="C4" s="20">
         <v>43984</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4" s="17"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="29"/>
+      <c r="H4" s="23"/>
       <c r="I4" s="30"/>
       <c r="J4" s="30"/>
     </row>
-    <row r="5" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="24"/>
+    <row r="5" spans="3:10" ht="15" customHeight="1">
+      <c r="C5" s="21"/>
       <c r="D5" s="16"/>
       <c r="E5" s="17"/>
       <c r="G5" s="11"/>
-      <c r="H5" s="29"/>
+      <c r="H5" s="23"/>
       <c r="I5" s="30"/>
       <c r="J5" s="30"/>
     </row>
-    <row r="6" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:10" ht="15" customHeight="1">
       <c r="C6" s="3" t="str">
         <f>IFERROR(DateVal+1,"")</f>
         <v/>
@@ -3042,157 +3059,157 @@
       <c r="D6" s="16"/>
       <c r="E6" s="17"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="20"/>
-    </row>
-    <row r="7" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="28"/>
+    </row>
+    <row r="7" spans="3:10" ht="15" customHeight="1">
       <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="17"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-    </row>
-    <row r="8" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="22"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+    </row>
+    <row r="8" spans="3:10" ht="15" customHeight="1">
       <c r="C8" s="2"/>
       <c r="D8" s="18"/>
       <c r="E8" s="19"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-    </row>
-    <row r="9" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="22"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+    </row>
+    <row r="9" spans="3:10" ht="15" customHeight="1">
       <c r="C9" s="8" t="str">
         <f>IFERROR(TEXT(DATEVALUE(DateVal)+2,"dddd"),"")</f>
         <v/>
       </c>
       <c r="D9" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E9" s="15"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="20"/>
-    </row>
-    <row r="10" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="23">
+      <c r="H9" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="28"/>
+    </row>
+    <row r="10" spans="3:10" ht="15" customHeight="1">
+      <c r="C10" s="20">
         <v>43985</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E10" s="17"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-    </row>
-    <row r="11" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="24"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+    </row>
+    <row r="11" spans="3:10" ht="15" customHeight="1">
+      <c r="C11" s="21"/>
       <c r="D11" s="16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E11" s="17"/>
       <c r="G11" s="11"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-    </row>
-    <row r="12" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="22"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+    </row>
+    <row r="12" spans="3:10" ht="15" customHeight="1">
       <c r="C12" s="3" t="str">
         <f>IFERROR(DateVal+2,"")</f>
         <v/>
       </c>
       <c r="D12" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E12" s="17"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="J12" s="20"/>
-    </row>
-    <row r="13" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="28"/>
+    </row>
+    <row r="13" spans="3:10" ht="15" customHeight="1">
       <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="17"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-    </row>
-    <row r="14" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="22"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+    </row>
+    <row r="14" spans="3:10" ht="15" customHeight="1">
       <c r="C14" s="2"/>
       <c r="D14" s="18"/>
       <c r="E14" s="19"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-    </row>
-    <row r="15" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="22"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+    </row>
+    <row r="15" spans="3:10" ht="15" customHeight="1">
       <c r="C15" s="8" t="str">
         <f>IFERROR(TEXT(DATEVALUE(DateVal)+3,"dddd"),"")</f>
         <v/>
       </c>
       <c r="D15" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E15" s="15"/>
       <c r="G15" s="9"/>
-      <c r="H15" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I15" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="20"/>
-    </row>
-    <row r="16" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="23">
+      <c r="H15" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="28"/>
+    </row>
+    <row r="16" spans="3:10" ht="15" customHeight="1">
+      <c r="C16" s="20">
         <v>43986</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" s="17"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-    </row>
-    <row r="17" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="24"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+    </row>
+    <row r="17" spans="3:10" ht="15" customHeight="1">
+      <c r="C17" s="21"/>
       <c r="D17" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17" s="17"/>
       <c r="G17" s="11"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-    </row>
-    <row r="18" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="22"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+    </row>
+    <row r="18" spans="3:10" ht="15" customHeight="1">
       <c r="C18" s="3" t="str">
         <f>IFERROR(DateVal+3,"")</f>
         <v/>
@@ -3200,343 +3217,367 @@
       <c r="D18" s="16"/>
       <c r="E18" s="17"/>
       <c r="G18" s="9"/>
-      <c r="H18" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="J18" s="20"/>
-    </row>
-    <row r="19" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="28"/>
+    </row>
+    <row r="19" spans="3:10" ht="15" customHeight="1">
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="17"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-    </row>
-    <row r="20" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="22"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+    </row>
+    <row r="20" spans="3:10" ht="15" customHeight="1">
       <c r="C20" s="2"/>
       <c r="D20" s="18"/>
       <c r="E20" s="19"/>
       <c r="G20" s="11"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-    </row>
-    <row r="21" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="22"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+    </row>
+    <row r="21" spans="3:10" ht="15" customHeight="1">
       <c r="C21" s="8" t="str">
         <f>IFERROR(TEXT(DATEVALUE(DateVal)+4,"dddd"),"")</f>
         <v/>
       </c>
       <c r="D21" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E21" s="15"/>
       <c r="G21" s="9"/>
-      <c r="H21" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="J21" s="20"/>
-    </row>
-    <row r="22" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="23">
+      <c r="H21" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21" s="28"/>
+    </row>
+    <row r="22" spans="3:10" ht="15" customHeight="1">
+      <c r="C22" s="20">
         <v>43987</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E22" s="17"/>
       <c r="G22" s="7"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-    </row>
-    <row r="23" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="24"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+    </row>
+    <row r="23" spans="3:10" ht="15" customHeight="1">
+      <c r="C23" s="21"/>
       <c r="D23" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E23" s="17"/>
       <c r="G23" s="11"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-    </row>
-    <row r="24" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H23" s="22"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+    </row>
+    <row r="24" spans="3:10" ht="15" customHeight="1">
       <c r="C24" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E24" s="17"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="J24" s="20"/>
-    </row>
-    <row r="25" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="J24" s="28"/>
+    </row>
+    <row r="25" spans="3:10" ht="15" customHeight="1">
       <c r="C25" s="2"/>
       <c r="D25" s="18"/>
       <c r="E25" s="19"/>
       <c r="G25" s="7"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-    </row>
-    <row r="26" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H25" s="22"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="28"/>
+    </row>
+    <row r="26" spans="3:10" ht="15" customHeight="1">
       <c r="C26" s="8" t="str">
         <f>IFERROR(TEXT(DATEVALUE(DateVal)+5,"dddd"),"")</f>
         <v/>
       </c>
       <c r="E26" s="15"/>
       <c r="G26" s="11"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-    </row>
-    <row r="27" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="23">
+      <c r="H26" s="22"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+    </row>
+    <row r="27" spans="3:10" ht="15" customHeight="1">
+      <c r="C27" s="20">
         <v>43988</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="17"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="J27" s="20"/>
-    </row>
-    <row r="28" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="24"/>
+      <c r="H27" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="I27" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="J27" s="28"/>
+    </row>
+    <row r="28" spans="3:10" ht="15" customHeight="1">
+      <c r="C28" s="21"/>
       <c r="D28" s="16"/>
       <c r="E28" s="17"/>
       <c r="G28" s="7"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-    </row>
-    <row r="29" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="22"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+    </row>
+    <row r="29" spans="3:10" ht="15" customHeight="1">
       <c r="C29" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="17"/>
       <c r="G29" s="11"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-    </row>
-    <row r="30" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H29" s="22"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+    </row>
+    <row r="30" spans="3:10" ht="15" customHeight="1">
       <c r="C30" s="2"/>
       <c r="D30" s="18"/>
       <c r="E30" s="19"/>
       <c r="G30" s="9"/>
-      <c r="H30" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="J30" s="20"/>
-    </row>
-    <row r="31" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H30" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J30" s="28"/>
+    </row>
+    <row r="31" spans="3:10" ht="15" customHeight="1">
       <c r="C31" s="8" t="str">
         <f>IFERROR(TEXT(DATEVALUE(DateVal)+6,"dddd"),"")</f>
         <v/>
       </c>
-      <c r="D31" s="25" t="str">
+      <c r="D31" s="24" t="str">
         <f>IFERROR(INDEX(#REF!,MATCH($C$34&amp;"|"&amp;ROW(A1),#REF!,0),2),"")</f>
         <v/>
       </c>
-      <c r="E31" s="26"/>
+      <c r="E31" s="25"/>
       <c r="G31" s="7"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-    </row>
-    <row r="32" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="23">
+      <c r="H31" s="22"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+    </row>
+    <row r="32" spans="3:10" ht="15" customHeight="1">
+      <c r="C32" s="20">
         <v>43989</v>
       </c>
-      <c r="D32" s="27"/>
-      <c r="E32" s="28"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="27"/>
       <c r="G32" s="11"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-    </row>
-    <row r="33" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="24"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="28"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+    </row>
+    <row r="33" spans="3:10" ht="15" customHeight="1">
+      <c r="C33" s="21"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="27"/>
       <c r="G33" s="9"/>
-      <c r="H33" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="I33" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="J33" s="20"/>
-    </row>
-    <row r="34" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H33" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="J33" s="28"/>
+    </row>
+    <row r="34" spans="3:10" ht="15" customHeight="1">
       <c r="C34" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="27"/>
-      <c r="E34" s="28"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="27"/>
       <c r="G34" s="7"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-    </row>
-    <row r="35" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H34" s="22"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+    </row>
+    <row r="35" spans="3:10" ht="15" customHeight="1">
       <c r="C35" s="2"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="28"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="27"/>
       <c r="G35" s="11"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-    </row>
-    <row r="36" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H35" s="22"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
+    </row>
+    <row r="36" spans="3:10" ht="15" customHeight="1">
       <c r="G36" s="10"/>
-      <c r="H36" s="29" t="s">
-        <v>19</v>
+      <c r="H36" s="23" t="s">
+        <v>17</v>
       </c>
       <c r="I36" s="30" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J36" s="30"/>
     </row>
-    <row r="37" spans="3:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:10" ht="13.5" customHeight="1">
       <c r="G37" s="7"/>
-      <c r="H37" s="29"/>
+      <c r="H37" s="23"/>
       <c r="I37" s="30"/>
       <c r="J37" s="30"/>
     </row>
-    <row r="38" spans="3:10" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:10" ht="23.25">
       <c r="G38" s="11"/>
-      <c r="H38" s="29"/>
+      <c r="H38" s="23"/>
       <c r="I38" s="30"/>
       <c r="J38" s="30"/>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:10">
       <c r="F39" s="4"/>
       <c r="G39" s="10"/>
-      <c r="H39" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I39" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="J39" s="20"/>
-    </row>
-    <row r="40" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H39" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="J39" s="28"/>
+    </row>
+    <row r="40" spans="3:10" ht="15" customHeight="1">
       <c r="F40" s="4"/>
       <c r="G40" s="7"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-    </row>
-    <row r="41" spans="3:10" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="H40" s="22"/>
+      <c r="I40" s="28"/>
+      <c r="J40" s="28"/>
+    </row>
+    <row r="41" spans="3:10" ht="23.25">
       <c r="F41" s="4"/>
       <c r="G41" s="11"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-    </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H41" s="22"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="28"/>
+    </row>
+    <row r="42" spans="3:10">
       <c r="F42" s="4"/>
       <c r="G42" s="10"/>
-      <c r="H42" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="I42" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="J42" s="20"/>
-    </row>
-    <row r="43" spans="3:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H42" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="I42" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J42" s="28"/>
+    </row>
+    <row r="43" spans="3:10" ht="14.25" customHeight="1">
       <c r="F43" s="4"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-    </row>
-    <row r="44" spans="3:10" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="H43" s="22"/>
+      <c r="I43" s="28"/>
+      <c r="J43" s="28"/>
+    </row>
+    <row r="44" spans="3:10" ht="23.25">
       <c r="F44" s="4"/>
       <c r="G44" s="11"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-    </row>
-    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H44" s="22"/>
+      <c r="I44" s="28"/>
+      <c r="J44" s="28"/>
+    </row>
+    <row r="45" spans="3:10">
       <c r="F45" s="4"/>
       <c r="G45" s="10"/>
-      <c r="H45" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="I45" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="J45" s="20"/>
-    </row>
-    <row r="46" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H45" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I45" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="J45" s="28"/>
+    </row>
+    <row r="46" spans="3:10" ht="15.75" customHeight="1">
       <c r="F46" s="4"/>
       <c r="G46" s="7"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
-    </row>
-    <row r="47" spans="3:10" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="H46" s="22"/>
+      <c r="I46" s="28"/>
+      <c r="J46" s="28"/>
+    </row>
+    <row r="47" spans="3:10" ht="23.25">
       <c r="F47" s="4"/>
       <c r="G47" s="11"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-    </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H47" s="22"/>
+      <c r="I47" s="28"/>
+      <c r="J47" s="28"/>
+    </row>
+    <row r="48" spans="3:10">
       <c r="G48" s="10"/>
-      <c r="H48" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="I48" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="J48" s="20"/>
-    </row>
-    <row r="49" spans="7:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H48" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I48" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J48" s="28"/>
+    </row>
+    <row r="49" spans="7:10" ht="15.75" customHeight="1">
       <c r="G49" s="7"/>
-      <c r="H49" s="21"/>
-      <c r="I49" s="20"/>
-      <c r="J49" s="20"/>
-    </row>
-    <row r="50" spans="7:10" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="H49" s="22"/>
+      <c r="I49" s="28"/>
+      <c r="J49" s="28"/>
+    </row>
+    <row r="50" spans="7:10" ht="23.25">
       <c r="G50" s="11"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="20"/>
-    </row>
-    <row r="51" spans="7:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="7:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="28"/>
+      <c r="J50" s="28"/>
+    </row>
+    <row r="51" spans="7:10" ht="15" customHeight="1"/>
+    <row r="52" spans="7:10" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J5"/>
+    <mergeCell ref="I6:J8"/>
+    <mergeCell ref="I9:J11"/>
+    <mergeCell ref="I12:J14"/>
+    <mergeCell ref="H42:H44"/>
+    <mergeCell ref="I42:J44"/>
+    <mergeCell ref="I45:J47"/>
+    <mergeCell ref="I48:J50"/>
+    <mergeCell ref="H48:H50"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="I33:J35"/>
+    <mergeCell ref="I39:J41"/>
+    <mergeCell ref="H36:H38"/>
+    <mergeCell ref="H39:H41"/>
+    <mergeCell ref="I18:J20"/>
+    <mergeCell ref="I15:J17"/>
+    <mergeCell ref="I21:J23"/>
+    <mergeCell ref="I24:J26"/>
+    <mergeCell ref="I27:J29"/>
+    <mergeCell ref="I30:J32"/>
+    <mergeCell ref="I36:J38"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="H18:H20"/>
     <mergeCell ref="H3:H5"/>
@@ -3553,30 +3594,6 @@
     <mergeCell ref="H24:H26"/>
     <mergeCell ref="H27:H29"/>
     <mergeCell ref="H30:H32"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="I33:J35"/>
-    <mergeCell ref="I39:J41"/>
-    <mergeCell ref="H36:H38"/>
-    <mergeCell ref="H39:H41"/>
-    <mergeCell ref="H42:H44"/>
-    <mergeCell ref="I42:J44"/>
-    <mergeCell ref="I45:J47"/>
-    <mergeCell ref="I48:J50"/>
-    <mergeCell ref="H48:H50"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J5"/>
-    <mergeCell ref="I6:J8"/>
-    <mergeCell ref="I9:J11"/>
-    <mergeCell ref="I12:J14"/>
-    <mergeCell ref="I18:J20"/>
-    <mergeCell ref="I15:J17"/>
-    <mergeCell ref="I21:J23"/>
-    <mergeCell ref="I24:J26"/>
-    <mergeCell ref="I27:J29"/>
-    <mergeCell ref="I30:J32"/>
-    <mergeCell ref="I36:J38"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Notes or To Do list in this column" sqref="H2"/>
@@ -3609,6 +3626,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a8a52e8c320b9a064ae3583ae3861c92">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88020cb39231a0945110f9cd888b521a" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -3829,15 +3855,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71FCDC0B-BE17-4EFD-AAD5-1E4E9349882C}">
   <ds:schemaRefs>
@@ -3856,6 +3873,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19F07B9F-2027-487B-9D1F-78CE832B31AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47490C6C-6B46-4DFD-9ACA-031AB2832B8C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3872,12 +3897,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19F07B9F-2027-487B-9D1F-78CE832B31AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>